<commit_message>
Ingreso: cabecera compra, masivo con compra y proveedores auto-upsert
</commit_message>
<xml_diff>
--- a/public/plantilla_ingreso_epp.xlsx
+++ b/public/plantilla_ingreso_epp.xlsx
@@ -124,37 +124,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/comments/comment1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>EPP Control</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
-      <text>
-        <t>Seleccione una categoría desde la lista</t>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
-      <text>
-        <t>Cantidad numérica mayor a 0</t>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
-      <text>
-        <t>Monto unitario SIN puntos ni comas. Ejemplo válido: 15990
-Ejemplo inválido: 15.990 / 15,990</t>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
-      <text>
-        <t>Seleccione desde la lista desplegable</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -444,13 +413,27 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="28" customWidth="1" min="2" max="2"/>
+    <col width="14" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="12" customWidth="1" min="9" max="9"/>
+    <col width="14" customWidth="1" min="10" max="10"/>
+    <col width="26" customWidth="1" min="11" max="11"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -483,23 +466,33 @@
           <t>Tipo IVA</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Tipo doc</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>N° documento</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Fecha doc</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>RUT proveedor</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Proveedor</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation sqref="A2:A101" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" error="Debe seleccionar una categoría válida" promptTitle="Categoría" prompt="Seleccione una categoría válida" type="list">
-      <formula1>"Cabeza,Ojos,Oídos,Vías respiratorias,Manos,Pies,Cuerpo,Altura,Otro"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2:D101" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" error="La cantidad debe ser un número entero mayor a 0" type="whole" operator="greaterThan">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation sqref="E2:E101" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" error="El monto debe ser un número entero sin puntos ni comas (ej: 15990)" type="custom">
-      <formula1>=AND(ISNUMBER(E2),INT(E2)=E2)</formula1>
-    </dataValidation>
-    <dataValidation sqref="F2:F101" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" error="Seleccione IVA incluido o + IVA" promptTitle="Tipo IVA" prompt="Seleccione IVA incluido o + IVA" type="list">
-      <formula1>"IVA incluido,+ IVA"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
</xml_diff>